<commit_message>
[UPDATE] - Selectors to fill jotform
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ornella.russo\Documents\UiPath\IngresoCedulas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBE948E-2733-485F-9814-F1D6B248BBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F52DC56-C8A9-4546-A0C9-7A086EBBED9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -162,9 +162,6 @@
     <t>ProcessABCQueue</t>
   </si>
   <si>
-    <t>https://form.jotform.com/230173673270654</t>
-  </si>
-  <si>
     <t>JotFormUrl</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>Data\Input\HTMLBody.txt</t>
+  </si>
+  <si>
+    <t>https://form.jotform.com/230235754449055</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -645,26 +645,26 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>